<commit_message>
fixes and input layers available
</commit_message>
<xml_diff>
--- a/ProcessingRiskPlugin/Excel_input_data/VEG_to_FUEL_TYPE.xlsx
+++ b/ProcessingRiskPlugin/Excel_input_data/VEG_to_FUEL_TYPE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giorg\AppData\Roaming\QGIS\QGIS3\profiles\default\python\plugins\ProcessingRiskPlugin\Excel_input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E367BD2-AE8A-43EC-A5A5-F8CDCB8D0462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE34F4E-903C-4D8B-8214-12914897B63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28320" yWindow="480" windowWidth="19410" windowHeight="11235" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,13 +45,13 @@
     <t>conifers</t>
   </si>
   <si>
-    <t>shurbs</t>
-  </si>
-  <si>
     <t>is_urban</t>
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>shrubs</t>
   </si>
 </sst>
 </file>
@@ -506,17 +506,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="1022" max="1024" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="1022" max="1024" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -524,10 +524,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>111</v>
       </c>
@@ -535,10 +535,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>112</v>
       </c>
@@ -546,10 +546,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>121</v>
       </c>
@@ -557,10 +557,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>122</v>
       </c>
@@ -568,10 +568,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>123</v>
       </c>
@@ -579,10 +579,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>124</v>
       </c>
@@ -590,10 +590,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>131</v>
       </c>
@@ -601,10 +601,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>132</v>
       </c>
@@ -612,10 +612,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>133</v>
       </c>
@@ -623,10 +623,10 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>141</v>
       </c>
@@ -634,10 +634,10 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>142</v>
       </c>
@@ -645,10 +645,10 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>211</v>
       </c>
@@ -656,7 +656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>212</v>
       </c>
@@ -664,7 +664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>213</v>
       </c>
@@ -672,7 +672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>221</v>
       </c>
@@ -680,7 +680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>222</v>
       </c>
@@ -688,7 +688,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>223</v>
       </c>
@@ -696,7 +696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>231</v>
       </c>
@@ -704,7 +704,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>241</v>
       </c>
@@ -712,7 +712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>242</v>
       </c>
@@ -720,7 +720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>243</v>
       </c>
@@ -728,7 +728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>244</v>
       </c>
@@ -736,7 +736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>311</v>
       </c>
@@ -744,7 +744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>312</v>
       </c>
@@ -752,7 +752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>313</v>
       </c>
@@ -760,7 +760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>321</v>
       </c>
@@ -768,31 +768,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>322</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>323</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>324</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>331</v>
       </c>
@@ -800,7 +800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>332</v>
       </c>
@@ -808,23 +808,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>333</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>334</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>335</v>
       </c>
@@ -832,7 +832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>411</v>
       </c>
@@ -840,7 +840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>412</v>
       </c>
@@ -848,7 +848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>421</v>
       </c>
@@ -856,7 +856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>422</v>
       </c>
@@ -864,7 +864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>423</v>
       </c>
@@ -872,7 +872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>511</v>
       </c>
@@ -880,7 +880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>512</v>
       </c>
@@ -888,7 +888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>521</v>
       </c>
@@ -896,7 +896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>522</v>
       </c>
@@ -904,7 +904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>523</v>
       </c>
@@ -912,7 +912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>999</v>
       </c>
@@ -920,7 +920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>0</v>
       </c>

</xml_diff>